<commit_message>
replace graph on my about for full html/css version close #1
</commit_message>
<xml_diff>
--- a/resources/Graphs.xlsx
+++ b/resources/Graphs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leo\Dev\RoosterGames\Site\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECE78E42-3CBA-4A7E-86AE-AC2D6477203F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB8E32A0-2567-49EC-9A74-1304391F588A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C4DC5210-D500-4B89-BAA5-D4BC934B66B7}"/>
+    <workbookView xWindow="-12495" yWindow="3420" windowWidth="11190" windowHeight="11295" xr2:uid="{C4DC5210-D500-4B89-BAA5-D4BC934B66B7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Category</t>
   </si>
@@ -60,6 +60,12 @@
   </si>
   <si>
     <t>Game Design</t>
+  </si>
+  <si>
+    <t>Total Members</t>
+  </si>
+  <si>
+    <t>Percentage</t>
   </si>
 </sst>
 </file>
@@ -101,9 +107,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -232,7 +240,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$2</c:f>
+              <c:f>Sheet1!$C$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -356,7 +364,7 @@
           </c:dPt>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$3:$B$8</c:f>
+              <c:f>Sheet1!$B$5:$B$10</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -382,7 +390,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$3:$C$8</c:f>
+              <c:f>Sheet1!$C$5:$C$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1196,15 +1204,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>100012</xdr:rowOff>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>147637</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>371475</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1549,59 +1557,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{817AD196-A92C-457B-8688-96E0F07E8C0E}">
-  <dimension ref="B2:M17"/>
+  <dimension ref="B2:M19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="29.28515625" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-    </row>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3">
         <v>8</v>
       </c>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
+      <c r="C2">
+        <v>19</v>
+      </c>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="1"/>
+      <c r="E4" s="2"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
@@ -1613,12 +1599,16 @@
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C5">
         <v>8</v>
       </c>
-      <c r="E5" s="1"/>
+      <c r="D5" s="3">
+        <f>(C5/$C$12)</f>
+        <v>0.21052631578947367</v>
+      </c>
+      <c r="E5" s="2"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
@@ -1630,12 +1620,16 @@
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C6">
-        <v>4</v>
-      </c>
-      <c r="E6" s="1"/>
+        <v>9</v>
+      </c>
+      <c r="D6" s="3">
+        <f t="shared" ref="D6:D10" si="0">(C6/$C$12)</f>
+        <v>0.23684210526315788</v>
+      </c>
+      <c r="E6" s="2"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
@@ -1647,12 +1641,16 @@
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C7">
-        <v>3</v>
-      </c>
-      <c r="E7" s="1"/>
+        <v>8</v>
+      </c>
+      <c r="D7" s="3">
+        <f t="shared" si="0"/>
+        <v>0.21052631578947367</v>
+      </c>
+      <c r="E7" s="2"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
@@ -1664,12 +1662,16 @@
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C8">
-        <v>6</v>
-      </c>
-      <c r="E8" s="1"/>
+        <v>4</v>
+      </c>
+      <c r="D8" s="3">
+        <f t="shared" si="0"/>
+        <v>0.10526315789473684</v>
+      </c>
+      <c r="E8" s="2"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
@@ -1680,7 +1682,17 @@
       <c r="M8" s="1"/>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="E9" s="1"/>
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9">
+        <v>3</v>
+      </c>
+      <c r="D9" s="3">
+        <f t="shared" si="0"/>
+        <v>7.8947368421052627E-2</v>
+      </c>
+      <c r="E9" s="2"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
@@ -1691,7 +1703,17 @@
       <c r="M9" s="1"/>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="E10" s="1"/>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10">
+        <v>6</v>
+      </c>
+      <c r="D10" s="3">
+        <f t="shared" si="0"/>
+        <v>0.15789473684210525</v>
+      </c>
+      <c r="E10" s="2"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
@@ -1702,7 +1724,7 @@
       <c r="M10" s="1"/>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="E11" s="1"/>
+      <c r="E11" s="2"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
@@ -1713,7 +1735,15 @@
       <c r="M11" s="1"/>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="E12" s="1"/>
+      <c r="C12">
+        <f>SUM(C5:C10)</f>
+        <v>38</v>
+      </c>
+      <c r="D12" s="3">
+        <f>SUM(D5:D10)</f>
+        <v>1</v>
+      </c>
+      <c r="E12" s="2"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
@@ -1724,7 +1754,7 @@
       <c r="M12" s="1"/>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="E13" s="1"/>
+      <c r="E13" s="2"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
@@ -1735,7 +1765,7 @@
       <c r="M13" s="1"/>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="E14" s="1"/>
+      <c r="E14" s="2"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
@@ -1746,7 +1776,7 @@
       <c r="M14" s="1"/>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="E15" s="1"/>
+      <c r="E15" s="2"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
@@ -1757,7 +1787,7 @@
       <c r="M15" s="1"/>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="E16" s="1"/>
+      <c r="E16" s="2"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
@@ -1768,7 +1798,7 @@
       <c r="M16" s="1"/>
     </row>
     <row r="17" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E17" s="1"/>
+      <c r="E17" s="2"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
@@ -1778,8 +1808,31 @@
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
     </row>
+    <row r="18" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="E18" s="2"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
+    </row>
+    <row r="19" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="E19" s="2"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+      <c r="M19" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>